<commit_message>
implentação de código que consegue ler todas as linhas da coluna Aparelho gela?
</commit_message>
<xml_diff>
--- a/planilhas/CCR (CBS).xlsx
+++ b/planilhas/CCR (CBS).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/paulo_kammer_ufsc_br/Documents/Área de Trabalho/Ar condicionado/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon\OneDrive\Documentos\GitHub\analisadorPlanilhas\planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3B7FDF7-5C3C-4107-AB70-1CEBD13051DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7351E6-242F-4F9E-A6BA-5211F3BBE48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{435BC634-9152-48F1-854E-F22B5DCECAAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{435BC634-9152-48F1-854E-F22B5DCECAAA}"/>
   </bookViews>
   <sheets>
     <sheet name="CURITIBANOS" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="140">
   <si>
     <t>PATRIMONIO</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>APARELHO</t>
+  </si>
+  <si>
+    <t>não</t>
+  </si>
+  <si>
+    <t>Aparelho gela?</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -507,11 +513,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,9 +540,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -541,9 +562,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -581,7 +602,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -687,7 +708,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -829,7 +850,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -837,11 +858,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E9596-56A8-40D0-A465-1682E1997EA5}">
-  <dimension ref="A1:H249"/>
+  <dimension ref="A1:I249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="L237" sqref="L237"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
@@ -851,9 +874,10 @@
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -878,8 +902,11 @@
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>193328</v>
       </c>
@@ -902,8 +929,9 @@
         <v>12000</v>
       </c>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>192835</v>
       </c>
@@ -926,8 +954,9 @@
         <v>18000</v>
       </c>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>192767</v>
       </c>
@@ -950,8 +979,9 @@
         <v>12000</v>
       </c>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>193299</v>
       </c>
@@ -974,8 +1004,9 @@
         <v>12000</v>
       </c>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>193297</v>
       </c>
@@ -998,8 +1029,9 @@
         <v>12000</v>
       </c>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>193298</v>
       </c>
@@ -1022,8 +1054,9 @@
         <v>12000</v>
       </c>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>193293</v>
       </c>
@@ -1046,8 +1079,9 @@
         <v>12000</v>
       </c>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>193294</v>
       </c>
@@ -1070,8 +1104,9 @@
         <v>12000</v>
       </c>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>193295</v>
       </c>
@@ -1094,8 +1129,9 @@
         <v>12000</v>
       </c>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>193296</v>
       </c>
@@ -1118,8 +1154,9 @@
         <v>12000</v>
       </c>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>193273</v>
       </c>
@@ -1142,8 +1179,9 @@
         <v>12000</v>
       </c>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>193283</v>
       </c>
@@ -1166,8 +1204,9 @@
         <v>12000</v>
       </c>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>193284</v>
       </c>
@@ -1190,8 +1229,9 @@
         <v>12000</v>
       </c>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>193285</v>
       </c>
@@ -1214,8 +1254,9 @@
         <v>12000</v>
       </c>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>192836</v>
       </c>
@@ -1238,8 +1279,9 @@
         <v>18000</v>
       </c>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>192837</v>
       </c>
@@ -1262,8 +1304,9 @@
         <v>18000</v>
       </c>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>193063</v>
       </c>
@@ -1288,8 +1331,11 @@
       <c r="H18" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>193064</v>
       </c>
@@ -1314,8 +1360,11 @@
       <c r="H19" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>193065</v>
       </c>
@@ -1338,8 +1387,9 @@
         <v>24000</v>
       </c>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>193266</v>
       </c>
@@ -1362,8 +1412,9 @@
         <v>12000</v>
       </c>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>193286</v>
       </c>
@@ -1386,8 +1437,9 @@
         <v>12000</v>
       </c>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>193062</v>
       </c>
@@ -1412,8 +1464,11 @@
       <c r="H23" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>193287</v>
       </c>
@@ -1436,8 +1491,9 @@
         <v>12000</v>
       </c>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>193288</v>
       </c>
@@ -1460,8 +1516,9 @@
         <v>12000</v>
       </c>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>193282</v>
       </c>
@@ -1484,8 +1541,9 @@
         <v>12000</v>
       </c>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>193289</v>
       </c>
@@ -1508,8 +1566,9 @@
         <v>12000</v>
       </c>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>193281</v>
       </c>
@@ -1532,8 +1591,9 @@
         <v>12000</v>
       </c>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>193290</v>
       </c>
@@ -1556,8 +1616,9 @@
         <v>12000</v>
       </c>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>193280</v>
       </c>
@@ -1580,8 +1641,9 @@
         <v>12000</v>
       </c>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>193291</v>
       </c>
@@ -1604,8 +1666,9 @@
         <v>12000</v>
       </c>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>193279</v>
       </c>
@@ -1628,8 +1691,9 @@
         <v>12000</v>
       </c>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>193292</v>
       </c>
@@ -1652,8 +1716,9 @@
         <v>12000</v>
       </c>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>193278</v>
       </c>
@@ -1676,8 +1741,9 @@
         <v>12000</v>
       </c>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>193302</v>
       </c>
@@ -1700,8 +1766,9 @@
         <v>12000</v>
       </c>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>193277</v>
       </c>
@@ -1724,8 +1791,9 @@
         <v>12000</v>
       </c>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>193301</v>
       </c>
@@ -1748,8 +1816,9 @@
         <v>12000</v>
       </c>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>193276</v>
       </c>
@@ -1772,8 +1841,9 @@
         <v>12000</v>
       </c>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>193300</v>
       </c>
@@ -1796,8 +1866,9 @@
         <v>12000</v>
       </c>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>193275</v>
       </c>
@@ -1820,8 +1891,9 @@
         <v>12000</v>
       </c>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>193274</v>
       </c>
@@ -1844,8 +1916,9 @@
         <v>12000</v>
       </c>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>192766</v>
       </c>
@@ -1868,8 +1941,9 @@
         <v>12000</v>
       </c>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>192838</v>
       </c>
@@ -1892,8 +1966,9 @@
         <v>18000</v>
       </c>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>193307</v>
       </c>
@@ -1916,8 +1991,9 @@
         <v>12000</v>
       </c>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>193308</v>
       </c>
@@ -1942,8 +2018,11 @@
       <c r="H45" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>193309</v>
       </c>
@@ -1968,8 +2047,11 @@
       <c r="H46" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>193305</v>
       </c>
@@ -1992,8 +2074,9 @@
         <v>12000</v>
       </c>
       <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>193306</v>
       </c>
@@ -2016,8 +2099,9 @@
         <v>22000</v>
       </c>
       <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>193304</v>
       </c>
@@ -2042,8 +2126,9 @@
       <c r="H49" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>193303</v>
       </c>
@@ -2068,8 +2153,9 @@
       <c r="H50" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>193327</v>
       </c>
@@ -2092,8 +2178,9 @@
         <v>12000</v>
       </c>
       <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>393197</v>
       </c>
@@ -2116,8 +2203,9 @@
         <v>18000</v>
       </c>
       <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>391032</v>
       </c>
@@ -2140,8 +2228,9 @@
         <v>12000</v>
       </c>
       <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="1" t="s">
         <v>77</v>
@@ -2162,8 +2251,9 @@
         <v>30000</v>
       </c>
       <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="1" t="s">
         <v>77</v>
@@ -2184,8 +2274,9 @@
         <v>30000</v>
       </c>
       <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="1" t="s">
         <v>77</v>
@@ -2206,8 +2297,9 @@
         <v>30000</v>
       </c>
       <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="1" t="s">
         <v>77</v>
@@ -2228,8 +2320,9 @@
         <v>30000</v>
       </c>
       <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="1" t="s">
         <v>77</v>
@@ -2250,8 +2343,9 @@
         <v>30000</v>
       </c>
       <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="1" t="s">
         <v>77</v>
@@ -2272,8 +2366,9 @@
         <v>30000</v>
       </c>
       <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="1" t="s">
         <v>77</v>
@@ -2294,8 +2389,9 @@
         <v>30000</v>
       </c>
       <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="1" t="s">
         <v>77</v>
@@ -2316,8 +2412,9 @@
         <v>30000</v>
       </c>
       <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="1" t="s">
         <v>77</v>
@@ -2338,8 +2435,9 @@
         <v>30000</v>
       </c>
       <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="1" t="s">
         <v>92</v>
@@ -2356,8 +2454,9 @@
         <v>18000</v>
       </c>
       <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="1" t="s">
         <v>92</v>
@@ -2374,8 +2473,9 @@
         <v>18000</v>
       </c>
       <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="1" t="s">
         <v>92</v>
@@ -2392,8 +2492,9 @@
         <v>18000</v>
       </c>
       <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="1" t="s">
         <v>92</v>
@@ -2410,8 +2511,9 @@
         <v>18000</v>
       </c>
       <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="1" t="s">
         <v>92</v>
@@ -2428,8 +2530,9 @@
         <v>18000</v>
       </c>
       <c r="H67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="1" t="s">
         <v>92</v>
@@ -2446,8 +2549,9 @@
         <v>18000</v>
       </c>
       <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="1" t="s">
         <v>92</v>
@@ -2464,8 +2568,9 @@
         <v>18000</v>
       </c>
       <c r="H69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="1" t="s">
         <v>92</v>
@@ -2482,8 +2587,9 @@
         <v>18000</v>
       </c>
       <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="1" t="s">
         <v>92</v>
@@ -2500,8 +2606,9 @@
         <v>18000</v>
       </c>
       <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="1" t="s">
         <v>92</v>
@@ -2518,8 +2625,9 @@
         <v>18000</v>
       </c>
       <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="1" t="s">
         <v>92</v>
@@ -2536,8 +2644,9 @@
         <v>18000</v>
       </c>
       <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="1" t="s">
         <v>92</v>
@@ -2554,8 +2663,9 @@
         <v>18000</v>
       </c>
       <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="1" t="s">
         <v>92</v>
@@ -2572,8 +2682,9 @@
         <v>18000</v>
       </c>
       <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="1" t="s">
         <v>92</v>
@@ -2590,8 +2701,9 @@
         <v>18000</v>
       </c>
       <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="1" t="s">
         <v>92</v>
@@ -2608,8 +2720,9 @@
         <v>18000</v>
       </c>
       <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="1" t="s">
         <v>92</v>
@@ -2626,8 +2739,9 @@
         <v>18000</v>
       </c>
       <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="1" t="s">
         <v>92</v>
@@ -2644,8 +2758,9 @@
         <v>18000</v>
       </c>
       <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="1" t="s">
         <v>92</v>
@@ -2662,8 +2777,9 @@
         <v>18000</v>
       </c>
       <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="1" t="s">
         <v>92</v>
@@ -2680,8 +2796,9 @@
         <v>18000</v>
       </c>
       <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="1" t="s">
         <v>92</v>
@@ -2698,8 +2815,9 @@
         <v>18000</v>
       </c>
       <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="1" t="s">
         <v>92</v>
@@ -2716,8 +2834,9 @@
         <v>18000</v>
       </c>
       <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="1" t="s">
         <v>92</v>
@@ -2734,8 +2853,9 @@
         <v>18000</v>
       </c>
       <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="1" t="s">
         <v>92</v>
@@ -2752,8 +2872,9 @@
         <v>18000</v>
       </c>
       <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="1" t="s">
         <v>92</v>
@@ -2770,8 +2891,9 @@
         <v>18000</v>
       </c>
       <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="1" t="s">
         <v>92</v>
@@ -2788,8 +2910,9 @@
         <v>18000</v>
       </c>
       <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="1" t="s">
         <v>92</v>
@@ -2806,8 +2929,9 @@
         <v>18000</v>
       </c>
       <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="1" t="s">
         <v>92</v>
@@ -2824,8 +2948,9 @@
         <v>18000</v>
       </c>
       <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="1" t="s">
         <v>92</v>
@@ -2842,8 +2967,9 @@
         <v>18000</v>
       </c>
       <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="1" t="s">
         <v>92</v>
@@ -2860,8 +2986,9 @@
         <v>18000</v>
       </c>
       <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="1" t="s">
         <v>92</v>
@@ -2878,8 +3005,9 @@
         <v>18000</v>
       </c>
       <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="1" t="s">
         <v>92</v>
@@ -2896,8 +3024,9 @@
         <v>18000</v>
       </c>
       <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="1" t="s">
         <v>92</v>
@@ -2914,8 +3043,9 @@
         <v>18000</v>
       </c>
       <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="1" t="s">
         <v>92</v>
@@ -2932,8 +3062,9 @@
         <v>18000</v>
       </c>
       <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="1" t="s">
         <v>92</v>
@@ -2950,8 +3081,9 @@
         <v>24000</v>
       </c>
       <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="1" t="s">
         <v>92</v>
@@ -2968,8 +3100,9 @@
         <v>24000</v>
       </c>
       <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="1" t="s">
         <v>92</v>
@@ -2986,8 +3119,9 @@
         <v>24000</v>
       </c>
       <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="1" t="s">
         <v>92</v>
@@ -3004,8 +3138,9 @@
         <v>24000</v>
       </c>
       <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="1" t="s">
         <v>92</v>
@@ -3022,8 +3157,9 @@
         <v>24000</v>
       </c>
       <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="1" t="s">
         <v>92</v>
@@ -3040,8 +3176,9 @@
         <v>24000</v>
       </c>
       <c r="H101" s="1"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="1" t="s">
         <v>92</v>
@@ -3058,8 +3195,9 @@
         <v>24000</v>
       </c>
       <c r="H102" s="1"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="1" t="s">
         <v>92</v>
@@ -3076,8 +3214,9 @@
         <v>24000</v>
       </c>
       <c r="H103" s="1"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="1" t="s">
         <v>92</v>
@@ -3094,8 +3233,9 @@
         <v>24000</v>
       </c>
       <c r="H104" s="1"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="1" t="s">
         <v>92</v>
@@ -3112,8 +3252,9 @@
         <v>24000</v>
       </c>
       <c r="H105" s="1"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="1" t="s">
         <v>92</v>
@@ -3130,8 +3271,9 @@
         <v>24000</v>
       </c>
       <c r="H106" s="1"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="1"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="1" t="s">
         <v>92</v>
@@ -3148,8 +3290,9 @@
         <v>24000</v>
       </c>
       <c r="H107" s="1"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="1"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="1" t="s">
         <v>92</v>
@@ -3166,8 +3309,9 @@
         <v>24000</v>
       </c>
       <c r="H108" s="1"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="1" t="s">
         <v>92</v>
@@ -3184,8 +3328,9 @@
         <v>24000</v>
       </c>
       <c r="H109" s="1"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="1" t="s">
         <v>92</v>
@@ -3202,8 +3347,9 @@
         <v>24000</v>
       </c>
       <c r="H110" s="1"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="1" t="s">
         <v>92</v>
@@ -3220,8 +3366,9 @@
         <v>24000</v>
       </c>
       <c r="H111" s="1"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="1"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="1" t="s">
         <v>92</v>
@@ -3238,8 +3385,9 @@
         <v>24000</v>
       </c>
       <c r="H112" s="1"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="1"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="1" t="s">
         <v>92</v>
@@ -3256,8 +3404,9 @@
         <v>24000</v>
       </c>
       <c r="H113" s="1"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="1" t="s">
         <v>92</v>
@@ -3274,8 +3423,9 @@
         <v>36000</v>
       </c>
       <c r="H114" s="1"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="1" t="s">
         <v>92</v>
@@ -3292,8 +3442,9 @@
         <v>36000</v>
       </c>
       <c r="H115" s="1"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="1" t="s">
         <v>92</v>
@@ -3310,8 +3461,9 @@
         <v>36000</v>
       </c>
       <c r="H116" s="1"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="1" t="s">
         <v>92</v>
@@ -3328,8 +3480,9 @@
         <v>36000</v>
       </c>
       <c r="H117" s="1"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="1" t="s">
         <v>92</v>
@@ -3346,8 +3499,9 @@
         <v>36000</v>
       </c>
       <c r="H118" s="1"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="1" t="s">
         <v>92</v>
@@ -3364,8 +3518,9 @@
         <v>36000</v>
       </c>
       <c r="H119" s="1"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="1" t="s">
         <v>92</v>
@@ -3382,8 +3537,9 @@
         <v>36000</v>
       </c>
       <c r="H120" s="1"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="1" t="s">
         <v>92</v>
@@ -3400,8 +3556,9 @@
         <v>36000</v>
       </c>
       <c r="H121" s="1"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="1" t="s">
         <v>92</v>
@@ -3418,8 +3575,9 @@
         <v>36000</v>
       </c>
       <c r="H122" s="1"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="1" t="s">
         <v>92</v>
@@ -3436,8 +3594,9 @@
         <v>36000</v>
       </c>
       <c r="H123" s="1"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="1" t="s">
         <v>92</v>
@@ -3454,8 +3613,9 @@
         <v>36000</v>
       </c>
       <c r="H124" s="1"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="1" t="s">
         <v>92</v>
@@ -3472,8 +3632,9 @@
         <v>36000</v>
       </c>
       <c r="H125" s="1"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="1" t="s">
         <v>92</v>
@@ -3490,8 +3651,9 @@
         <v>36000</v>
       </c>
       <c r="H126" s="1"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="1" t="s">
         <v>92</v>
@@ -3508,8 +3670,9 @@
         <v>36000</v>
       </c>
       <c r="H127" s="1"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="1" t="s">
         <v>92</v>
@@ -3526,8 +3689,9 @@
         <v>36000</v>
       </c>
       <c r="H128" s="1"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="1"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="1" t="s">
         <v>92</v>
@@ -3544,8 +3708,9 @@
         <v>36000</v>
       </c>
       <c r="H129" s="1"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="1"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="1" t="s">
         <v>92</v>
@@ -3562,8 +3727,9 @@
         <v>36000</v>
       </c>
       <c r="H130" s="1"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="1"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="1" t="s">
         <v>92</v>
@@ -3580,8 +3746,9 @@
         <v>36000</v>
       </c>
       <c r="H131" s="1"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="1"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="1" t="s">
         <v>92</v>
@@ -3598,8 +3765,9 @@
         <v>36000</v>
       </c>
       <c r="H132" s="1"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="1"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="1" t="s">
         <v>92</v>
@@ -3616,8 +3784,9 @@
         <v>36000</v>
       </c>
       <c r="H133" s="1"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="1"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="1" t="s">
         <v>92</v>
@@ -3634,8 +3803,9 @@
         <v>36000</v>
       </c>
       <c r="H134" s="1"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="1"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="1" t="s">
         <v>92</v>
@@ -3652,8 +3822,9 @@
         <v>36000</v>
       </c>
       <c r="H135" s="1"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="1"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="1" t="s">
         <v>92</v>
@@ -3670,8 +3841,9 @@
         <v>36000</v>
       </c>
       <c r="H136" s="1"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="1"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="1" t="s">
         <v>92</v>
@@ -3688,8 +3860,9 @@
         <v>36000</v>
       </c>
       <c r="H137" s="1"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="1"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="1" t="s">
         <v>92</v>
@@ -3706,8 +3879,9 @@
         <v>36000</v>
       </c>
       <c r="H138" s="1"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="1"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="1" t="s">
         <v>92</v>
@@ -3724,8 +3898,9 @@
         <v>36000</v>
       </c>
       <c r="H139" s="1"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="1"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="1" t="s">
         <v>92</v>
@@ -3742,8 +3917,9 @@
         <v>36000</v>
       </c>
       <c r="H140" s="1"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="1"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="1" t="s">
         <v>92</v>
@@ -3760,8 +3936,9 @@
         <v>36000</v>
       </c>
       <c r="H141" s="1"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="1"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="1" t="s">
         <v>92</v>
@@ -3778,8 +3955,9 @@
         <v>36000</v>
       </c>
       <c r="H142" s="1"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="1"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="1" t="s">
         <v>92</v>
@@ -3796,8 +3974,9 @@
         <v>36000</v>
       </c>
       <c r="H143" s="1"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="1"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="1" t="s">
         <v>92</v>
@@ -3814,8 +3993,9 @@
         <v>36000</v>
       </c>
       <c r="H144" s="1"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="1"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3"/>
       <c r="B145" s="1" t="s">
         <v>92</v>
@@ -3832,8 +4012,9 @@
         <v>36000</v>
       </c>
       <c r="H145" s="1"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="1"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3"/>
       <c r="B146" s="1" t="s">
         <v>92</v>
@@ -3850,8 +4031,9 @@
         <v>36000</v>
       </c>
       <c r="H146" s="1"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="1"/>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3"/>
       <c r="B147" s="1" t="s">
         <v>92</v>
@@ -3868,8 +4050,9 @@
         <v>36000</v>
       </c>
       <c r="H147" s="1"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="1"/>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="1" t="s">
         <v>92</v>
@@ -3886,8 +4069,9 @@
         <v>36000</v>
       </c>
       <c r="H148" s="1"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="1"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="1" t="s">
         <v>92</v>
@@ -3904,8 +4088,9 @@
         <v>36000</v>
       </c>
       <c r="H149" s="1"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="1"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="1" t="s">
         <v>92</v>
@@ -3922,8 +4107,9 @@
         <v>36000</v>
       </c>
       <c r="H150" s="1"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="1"/>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="1" t="s">
         <v>92</v>
@@ -3940,8 +4126,9 @@
         <v>36000</v>
       </c>
       <c r="H151" s="1"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="1"/>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="1" t="s">
         <v>92</v>
@@ -3958,8 +4145,9 @@
         <v>36000</v>
       </c>
       <c r="H152" s="1"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="1"/>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="1" t="s">
         <v>92</v>
@@ -3976,8 +4164,9 @@
         <v>36000</v>
       </c>
       <c r="H153" s="1"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="1"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="1" t="s">
         <v>92</v>
@@ -3994,8 +4183,9 @@
         <v>36000</v>
       </c>
       <c r="H154" s="1"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="1"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="1" t="s">
         <v>92</v>
@@ -4012,8 +4202,9 @@
         <v>36000</v>
       </c>
       <c r="H155" s="1"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="1"/>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="1" t="s">
         <v>92</v>
@@ -4030,8 +4221,9 @@
         <v>36000</v>
       </c>
       <c r="H156" s="1"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="1"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3"/>
       <c r="B157" s="1" t="s">
         <v>92</v>
@@ -4048,8 +4240,9 @@
         <v>36000</v>
       </c>
       <c r="H157" s="1"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="1"/>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3"/>
       <c r="B158" s="1" t="s">
         <v>92</v>
@@ -4066,8 +4259,9 @@
         <v>36000</v>
       </c>
       <c r="H158" s="1"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="1"/>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3"/>
       <c r="B159" s="1" t="s">
         <v>92</v>
@@ -4084,8 +4278,9 @@
         <v>36000</v>
       </c>
       <c r="H159" s="1"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="1"/>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="3"/>
       <c r="B160" s="1" t="s">
         <v>92</v>
@@ -4102,8 +4297,9 @@
         <v>36000</v>
       </c>
       <c r="H160" s="1"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="1"/>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="3"/>
       <c r="B161" s="1" t="s">
         <v>92</v>
@@ -4120,8 +4316,9 @@
         <v>36000</v>
       </c>
       <c r="H161" s="1"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="1"/>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="3"/>
       <c r="B162" s="1" t="s">
         <v>92</v>
@@ -4138,8 +4335,9 @@
         <v>36000</v>
       </c>
       <c r="H162" s="1"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="1"/>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="3"/>
       <c r="B163" s="1" t="s">
         <v>92</v>
@@ -4156,8 +4354,9 @@
         <v>36000</v>
       </c>
       <c r="H163" s="1"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="1"/>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="3"/>
       <c r="B164" s="1" t="s">
         <v>92</v>
@@ -4174,8 +4373,9 @@
         <v>36000</v>
       </c>
       <c r="H164" s="1"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="1"/>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="3"/>
       <c r="B165" s="1" t="s">
         <v>92</v>
@@ -4192,8 +4392,9 @@
         <v>36000</v>
       </c>
       <c r="H165" s="1"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="1"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="3"/>
       <c r="B166" s="1" t="s">
         <v>92</v>
@@ -4210,8 +4411,9 @@
         <v>36000</v>
       </c>
       <c r="H166" s="1"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="1"/>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="3"/>
       <c r="B167" s="1" t="s">
         <v>92</v>
@@ -4228,8 +4430,9 @@
         <v>36000</v>
       </c>
       <c r="H167" s="1"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="1"/>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="3"/>
       <c r="B168" s="1" t="s">
         <v>92</v>
@@ -4246,8 +4449,9 @@
         <v>36000</v>
       </c>
       <c r="H168" s="1"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="1"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="3"/>
       <c r="B169" s="1" t="s">
         <v>92</v>
@@ -4264,8 +4468,9 @@
         <v>36000</v>
       </c>
       <c r="H169" s="1"/>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="1"/>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="3"/>
       <c r="B170" s="1" t="s">
         <v>92</v>
@@ -4282,8 +4487,9 @@
         <v>36000</v>
       </c>
       <c r="H170" s="1"/>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="1"/>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="3"/>
       <c r="B171" s="1" t="s">
         <v>92</v>
@@ -4300,8 +4506,9 @@
         <v>36000</v>
       </c>
       <c r="H171" s="1"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="1"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3"/>
       <c r="B172" s="1" t="s">
         <v>92</v>
@@ -4318,8 +4525,9 @@
         <v>36000</v>
       </c>
       <c r="H172" s="1"/>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="1"/>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="3"/>
       <c r="B173" s="1" t="s">
         <v>92</v>
@@ -4336,8 +4544,9 @@
         <v>24000</v>
       </c>
       <c r="H173" s="1"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="1"/>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="3"/>
       <c r="B174" s="1" t="s">
         <v>92</v>
@@ -4354,8 +4563,9 @@
         <v>24000</v>
       </c>
       <c r="H174" s="1"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="1"/>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="3"/>
       <c r="B175" s="1" t="s">
         <v>92</v>
@@ -4372,8 +4582,9 @@
         <v>24000</v>
       </c>
       <c r="H175" s="1"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="1"/>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="3"/>
       <c r="B176" s="1" t="s">
         <v>92</v>
@@ -4390,8 +4601,9 @@
         <v>24000</v>
       </c>
       <c r="H176" s="1"/>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="1"/>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="3"/>
       <c r="B177" s="1" t="s">
         <v>92</v>
@@ -4408,8 +4620,9 @@
         <v>12000</v>
       </c>
       <c r="H177" s="1"/>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="1"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="3"/>
       <c r="B178" s="1" t="s">
         <v>92</v>
@@ -4426,8 +4639,9 @@
         <v>12000</v>
       </c>
       <c r="H178" s="1"/>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="1"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="3"/>
       <c r="B179" s="1" t="s">
         <v>92</v>
@@ -4444,8 +4658,9 @@
         <v>12000</v>
       </c>
       <c r="H179" s="1"/>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="1"/>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="3"/>
       <c r="B180" s="1" t="s">
         <v>92</v>
@@ -4462,8 +4677,9 @@
         <v>12000</v>
       </c>
       <c r="H180" s="1"/>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="1"/>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="3"/>
       <c r="B181" s="1" t="s">
         <v>92</v>
@@ -4480,8 +4696,9 @@
         <v>12000</v>
       </c>
       <c r="H181" s="1"/>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" s="1"/>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="3"/>
       <c r="B182" s="1" t="s">
         <v>92</v>
@@ -4498,8 +4715,9 @@
         <v>12000</v>
       </c>
       <c r="H182" s="1"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="1"/>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="3"/>
       <c r="B183" s="1" t="s">
         <v>92</v>
@@ -4516,8 +4734,9 @@
         <v>12000</v>
       </c>
       <c r="H183" s="1"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="1"/>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="3"/>
       <c r="B184" s="1" t="s">
         <v>92</v>
@@ -4534,8 +4753,9 @@
         <v>12000</v>
       </c>
       <c r="H184" s="1"/>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" s="1"/>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="3"/>
       <c r="B185" s="1" t="s">
         <v>92</v>
@@ -4552,8 +4772,9 @@
         <v>12000</v>
       </c>
       <c r="H185" s="1"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="1"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="3"/>
       <c r="B186" s="1" t="s">
         <v>92</v>
@@ -4570,8 +4791,9 @@
         <v>12000</v>
       </c>
       <c r="H186" s="1"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" s="1"/>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="3"/>
       <c r="B187" s="1" t="s">
         <v>92</v>
@@ -4588,8 +4810,9 @@
         <v>12000</v>
       </c>
       <c r="H187" s="1"/>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="1"/>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="3"/>
       <c r="B188" s="1" t="s">
         <v>92</v>
@@ -4606,8 +4829,9 @@
         <v>12000</v>
       </c>
       <c r="H188" s="1"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="1"/>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="3"/>
       <c r="B189" s="1" t="s">
         <v>92</v>
@@ -4624,8 +4848,9 @@
         <v>12000</v>
       </c>
       <c r="H189" s="1"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="1"/>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="3"/>
       <c r="B190" s="1" t="s">
         <v>92</v>
@@ -4642,8 +4867,9 @@
         <v>12000</v>
       </c>
       <c r="H190" s="1"/>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="1"/>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="3"/>
       <c r="B191" s="1" t="s">
         <v>92</v>
@@ -4660,8 +4886,9 @@
         <v>12000</v>
       </c>
       <c r="H191" s="1"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="1"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="3"/>
       <c r="B192" s="1" t="s">
         <v>92</v>
@@ -4678,8 +4905,9 @@
         <v>12000</v>
       </c>
       <c r="H192" s="1"/>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" s="1"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="3"/>
       <c r="B193" s="1" t="s">
         <v>92</v>
@@ -4696,8 +4924,9 @@
         <v>12000</v>
       </c>
       <c r="H193" s="1"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" s="1"/>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="3"/>
       <c r="B194" s="1" t="s">
         <v>92</v>
@@ -4714,8 +4943,9 @@
         <v>12000</v>
       </c>
       <c r="H194" s="1"/>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I194" s="1"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="3"/>
       <c r="B195" s="1" t="s">
         <v>92</v>
@@ -4732,8 +4962,9 @@
         <v>12000</v>
       </c>
       <c r="H195" s="1"/>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I195" s="1"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="3"/>
       <c r="B196" s="1" t="s">
         <v>92</v>
@@ -4750,8 +4981,9 @@
         <v>9000</v>
       </c>
       <c r="H196" s="1"/>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I196" s="1"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="3"/>
       <c r="B197" s="1" t="s">
         <v>92</v>
@@ -4768,8 +5000,9 @@
         <v>9000</v>
       </c>
       <c r="H197" s="1"/>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I197" s="1"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="3"/>
       <c r="B198" s="1" t="s">
         <v>92</v>
@@ -4786,8 +5019,9 @@
         <v>9000</v>
       </c>
       <c r="H198" s="1"/>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I198" s="1"/>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="3"/>
       <c r="B199" s="1" t="s">
         <v>92</v>
@@ -4804,8 +5038,9 @@
         <v>9000</v>
       </c>
       <c r="H199" s="1"/>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I199" s="1"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="3"/>
       <c r="B200" s="1" t="s">
         <v>92</v>
@@ -4822,8 +5057,9 @@
         <v>9000</v>
       </c>
       <c r="H200" s="1"/>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I200" s="1"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="3"/>
       <c r="B201" s="1" t="s">
         <v>92</v>
@@ -4840,8 +5076,9 @@
         <v>9000</v>
       </c>
       <c r="H201" s="1"/>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I201" s="1"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="3"/>
       <c r="B202" s="1" t="s">
         <v>92</v>
@@ -4858,8 +5095,9 @@
         <v>9000</v>
       </c>
       <c r="H202" s="1"/>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" s="1"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="3"/>
       <c r="B203" s="1" t="s">
         <v>92</v>
@@ -4876,8 +5114,9 @@
         <v>9000</v>
       </c>
       <c r="H203" s="1"/>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I203" s="1"/>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="3"/>
       <c r="B204" s="1" t="s">
         <v>11</v>
@@ -4898,8 +5137,9 @@
         <v>30000</v>
       </c>
       <c r="H204" s="1"/>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I204" s="1"/>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
       <c r="B205" s="1" t="s">
         <v>11</v>
@@ -4920,8 +5160,9 @@
         <v>30000</v>
       </c>
       <c r="H205" s="1"/>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I205" s="1"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
       <c r="B206" s="1" t="s">
         <v>11</v>
@@ -4942,8 +5183,9 @@
         <v>30000</v>
       </c>
       <c r="H206" s="1"/>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I206" s="1"/>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
       <c r="B207" s="1" t="s">
         <v>11</v>
@@ -4964,8 +5206,9 @@
         <v>30000</v>
       </c>
       <c r="H207" s="1"/>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" s="1"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
       <c r="B208" s="1" t="s">
         <v>11</v>
@@ -4986,8 +5229,9 @@
         <v>30000</v>
       </c>
       <c r="H208" s="1"/>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I208" s="1"/>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>193319</v>
       </c>
@@ -5010,8 +5254,9 @@
         <v>12000</v>
       </c>
       <c r="H209" s="1"/>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I209" s="1"/>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>193326</v>
       </c>
@@ -5034,8 +5279,9 @@
         <v>12000</v>
       </c>
       <c r="H210" s="1"/>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I210" s="1"/>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>193321</v>
       </c>
@@ -5058,8 +5304,9 @@
         <v>12000</v>
       </c>
       <c r="H211" s="1"/>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I211" s="1"/>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>193322</v>
       </c>
@@ -5082,8 +5329,9 @@
         <v>12000</v>
       </c>
       <c r="H212" s="1"/>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I212" s="1"/>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>193323</v>
       </c>
@@ -5106,8 +5354,9 @@
         <v>12000</v>
       </c>
       <c r="H213" s="1"/>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I213" s="1"/>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>193324</v>
       </c>
@@ -5130,8 +5379,9 @@
         <v>12000</v>
       </c>
       <c r="H214" s="1"/>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I214" s="1"/>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>193325</v>
       </c>
@@ -5154,8 +5404,9 @@
         <v>12000</v>
       </c>
       <c r="H215" s="1"/>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I215" s="1"/>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="3"/>
       <c r="B216" s="1" t="s">
         <v>11</v>
@@ -5176,8 +5427,9 @@
         <v>30000</v>
       </c>
       <c r="H216" s="1"/>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I216" s="1"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="3"/>
       <c r="B217" s="1" t="s">
         <v>11</v>
@@ -5198,8 +5450,9 @@
         <v>30000</v>
       </c>
       <c r="H217" s="1"/>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I217" s="1"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="3"/>
       <c r="B218" s="1" t="s">
         <v>11</v>
@@ -5220,8 +5473,9 @@
         <v>30000</v>
       </c>
       <c r="H218" s="1"/>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I218" s="1"/>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="3"/>
       <c r="B219" s="1" t="s">
         <v>11</v>
@@ -5242,8 +5496,9 @@
         <v>30000</v>
       </c>
       <c r="H219" s="1"/>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I219" s="1"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>193316</v>
       </c>
@@ -5266,8 +5521,9 @@
         <v>12000</v>
       </c>
       <c r="H220" s="1"/>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I220" s="1"/>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="3">
         <v>193317</v>
       </c>
@@ -5290,8 +5546,9 @@
         <v>12000</v>
       </c>
       <c r="H221" s="1"/>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I221" s="1"/>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>193318</v>
       </c>
@@ -5314,8 +5571,9 @@
         <v>12000</v>
       </c>
       <c r="H222" s="1"/>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I222" s="1"/>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>193311</v>
       </c>
@@ -5338,8 +5596,9 @@
         <v>22000</v>
       </c>
       <c r="H223" s="1"/>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I223" s="1"/>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>193313</v>
       </c>
@@ -5362,8 +5621,9 @@
         <v>22000</v>
       </c>
       <c r="H224" s="1"/>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I224" s="1"/>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>193314</v>
       </c>
@@ -5386,8 +5646,9 @@
         <v>22000</v>
       </c>
       <c r="H225" s="1"/>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I225" s="1"/>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>193315</v>
       </c>
@@ -5410,8 +5671,9 @@
         <v>22000</v>
       </c>
       <c r="H226" s="1"/>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I226" s="1"/>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>193061</v>
       </c>
@@ -5434,8 +5696,9 @@
         <v>18000</v>
       </c>
       <c r="H227" s="1"/>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I227" s="1"/>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="3"/>
       <c r="B228" s="1" t="s">
         <v>11</v>
@@ -5456,8 +5719,9 @@
         <v>9000</v>
       </c>
       <c r="H228" s="1"/>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I228" s="1"/>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>192834</v>
       </c>
@@ -5480,8 +5744,9 @@
         <v>18000</v>
       </c>
       <c r="H229" s="1"/>
-    </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I229" s="1"/>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="3"/>
       <c r="B230" s="1" t="s">
         <v>11</v>
@@ -5502,8 +5767,9 @@
         <v>30000</v>
       </c>
       <c r="H230" s="1"/>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I230" s="1"/>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>192768</v>
       </c>
@@ -5528,8 +5794,11 @@
       <c r="H231" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I231" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="3"/>
       <c r="B232" s="1" t="s">
         <v>11</v>
@@ -5550,8 +5819,9 @@
         <v>12000</v>
       </c>
       <c r="H232" s="1"/>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I232" s="1"/>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="3"/>
       <c r="B233" s="1" t="s">
         <v>11</v>
@@ -5574,8 +5844,9 @@
       <c r="H233" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I233" s="1"/>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="3"/>
       <c r="B234" s="1" t="s">
         <v>11</v>
@@ -5598,8 +5869,9 @@
       <c r="H234" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I234" s="1"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="3"/>
       <c r="B235" s="1" t="s">
         <v>11</v>
@@ -5622,8 +5894,9 @@
       <c r="H235" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I235" s="1"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="1" t="s">
         <v>11</v>
@@ -5646,8 +5919,9 @@
       <c r="H236" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I236" s="1"/>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="1" t="s">
         <v>11</v>
@@ -5670,8 +5944,9 @@
       <c r="H237" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I237" s="1"/>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="1" t="s">
         <v>11</v>
@@ -5692,8 +5967,9 @@
         <v>9000</v>
       </c>
       <c r="H238" s="1"/>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I238" s="1"/>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
       <c r="B239" s="1" t="s">
         <v>11</v>
@@ -5714,8 +5990,9 @@
         <v>9000</v>
       </c>
       <c r="H239" s="1"/>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I239" s="1"/>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="1" t="s">
         <v>11</v>
@@ -5736,8 +6013,9 @@
         <v>9000</v>
       </c>
       <c r="H240" s="1"/>
-    </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I240" s="1"/>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="1" t="s">
         <v>11</v>
@@ -5760,8 +6038,9 @@
       <c r="H241" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I241" s="1"/>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="1" t="s">
         <v>11</v>
@@ -5782,8 +6061,9 @@
         <v>18000</v>
       </c>
       <c r="H242" s="1"/>
-    </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I242" s="1"/>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="1" t="s">
         <v>11</v>
@@ -5804,8 +6084,9 @@
         <v>9000</v>
       </c>
       <c r="H243" s="1"/>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I243" s="1"/>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="1" t="s">
         <v>11</v>
@@ -5826,8 +6107,9 @@
         <v>12000</v>
       </c>
       <c r="H244" s="1"/>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I244" s="1"/>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="1" t="s">
         <v>11</v>
@@ -5850,8 +6132,9 @@
       <c r="H245" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I245" s="1"/>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="1" t="s">
         <v>11</v>
@@ -5874,8 +6157,9 @@
       <c r="H246" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I246" s="1"/>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="1" t="s">
         <v>11</v>
@@ -5896,8 +6180,9 @@
         <v>18000</v>
       </c>
       <c r="H247" s="1"/>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I247" s="1"/>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="1" t="s">
         <v>11</v>
@@ -5918,8 +6203,9 @@
         <v>18000</v>
       </c>
       <c r="H248" s="1"/>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I248" s="1"/>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="1" t="s">
         <v>11</v>
@@ -5940,6 +6226,7 @@
         <v>22000</v>
       </c>
       <c r="H249" s="1"/>
+      <c r="I249" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H249">

</xml_diff>